<commit_message>
Tablas ajustadas, mejoras en AWS
</commit_message>
<xml_diff>
--- a/Proyecto/motorR/4098796/vecinos_ofertas_sin_asignar.xlsx
+++ b/Proyecto/motorR/4098796/vecinos_ofertas_sin_asignar.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
   <si>
     <t xml:space="preserve">job_id</t>
   </si>
@@ -20,126 +20,108 @@
     <t xml:space="preserve">vecinos</t>
   </si>
   <si>
+    <t xml:space="preserve">81</t>
+  </si>
+  <si>
+    <t xml:space="preserve">64</t>
+  </si>
+  <si>
+    <t xml:space="preserve">66</t>
+  </si>
+  <si>
+    <t xml:space="preserve">26</t>
+  </si>
+  <si>
+    <t xml:space="preserve">36</t>
+  </si>
+  <si>
+    <t xml:space="preserve">16</t>
+  </si>
+  <si>
+    <t xml:space="preserve">76</t>
+  </si>
+  <si>
+    <t xml:space="preserve">24</t>
+  </si>
+  <si>
+    <t xml:space="preserve">80</t>
+  </si>
+  <si>
+    <t xml:space="preserve">71</t>
+  </si>
+  <si>
     <t xml:space="preserve">56</t>
   </si>
   <si>
-    <t xml:space="preserve">64</t>
-  </si>
-  <si>
-    <t xml:space="preserve">66</t>
-  </si>
-  <si>
-    <t xml:space="preserve">26</t>
-  </si>
-  <si>
-    <t xml:space="preserve">36</t>
-  </si>
-  <si>
-    <t xml:space="preserve">16</t>
-  </si>
-  <si>
-    <t xml:space="preserve">76</t>
-  </si>
-  <si>
-    <t xml:space="preserve">24</t>
-  </si>
-  <si>
-    <t xml:space="preserve">80</t>
-  </si>
-  <si>
-    <t xml:space="preserve">83</t>
-  </si>
-  <si>
-    <t xml:space="preserve">6</t>
+    <t xml:space="preserve">68</t>
+  </si>
+  <si>
+    <t xml:space="preserve">54</t>
+  </si>
+  <si>
+    <t xml:space="preserve">33</t>
+  </si>
+  <si>
+    <t xml:space="preserve">78</t>
+  </si>
+  <si>
+    <t xml:space="preserve">22</t>
+  </si>
+  <si>
+    <t xml:space="preserve">50</t>
+  </si>
+  <si>
+    <t xml:space="preserve">29</t>
+  </si>
+  <si>
+    <t xml:space="preserve">67</t>
   </si>
   <si>
     <t xml:space="preserve">55</t>
   </si>
   <si>
-    <t xml:space="preserve">68</t>
-  </si>
-  <si>
-    <t xml:space="preserve">54</t>
-  </si>
-  <si>
-    <t xml:space="preserve">33</t>
-  </si>
-  <si>
-    <t xml:space="preserve">78</t>
-  </si>
-  <si>
-    <t xml:space="preserve">22</t>
-  </si>
-  <si>
-    <t xml:space="preserve">50</t>
-  </si>
-  <si>
-    <t xml:space="preserve">29</t>
-  </si>
-  <si>
-    <t xml:space="preserve">67</t>
-  </si>
-  <si>
-    <t xml:space="preserve">84</t>
-  </si>
-  <si>
-    <t xml:space="preserve">12</t>
+    <t xml:space="preserve">74</t>
+  </si>
+  <si>
+    <t xml:space="preserve">42</t>
+  </si>
+  <si>
+    <t xml:space="preserve">79</t>
+  </si>
+  <si>
+    <t xml:space="preserve">14</t>
+  </si>
+  <si>
+    <t xml:space="preserve">49</t>
+  </si>
+  <si>
+    <t xml:space="preserve">27</t>
   </si>
   <si>
     <t xml:space="preserve">63</t>
   </si>
   <si>
-    <t xml:space="preserve">74</t>
-  </si>
-  <si>
-    <t xml:space="preserve">79</t>
-  </si>
-  <si>
-    <t xml:space="preserve">14</t>
-  </si>
-  <si>
-    <t xml:space="preserve">49</t>
-  </si>
-  <si>
-    <t xml:space="preserve">27</t>
+    <t xml:space="preserve">60</t>
+  </si>
+  <si>
+    <t xml:space="preserve">72</t>
+  </si>
+  <si>
+    <t xml:space="preserve">30</t>
+  </si>
+  <si>
+    <t xml:space="preserve">13</t>
+  </si>
+  <si>
+    <t xml:space="preserve">44</t>
+  </si>
+  <si>
+    <t xml:space="preserve">51</t>
   </si>
   <si>
     <t xml:space="preserve">41</t>
   </si>
   <si>
-    <t xml:space="preserve">60</t>
-  </si>
-  <si>
-    <t xml:space="preserve">72</t>
-  </si>
-  <si>
-    <t xml:space="preserve">42</t>
-  </si>
-  <si>
-    <t xml:space="preserve">13</t>
-  </si>
-  <si>
-    <t xml:space="preserve">44</t>
-  </si>
-  <si>
-    <t xml:space="preserve">30</t>
-  </si>
-  <si>
-    <t xml:space="preserve">51</t>
-  </si>
-  <si>
-    <t xml:space="preserve">35</t>
-  </si>
-  <si>
-    <t xml:space="preserve">75</t>
-  </si>
-  <si>
-    <t xml:space="preserve">82</t>
-  </si>
-  <si>
-    <t xml:space="preserve">59</t>
-  </si>
-  <si>
     <t xml:space="preserve">46</t>
   </si>
   <si>
@@ -149,7 +131,7 @@
     <t xml:space="preserve">28</t>
   </si>
   <si>
-    <t xml:space="preserve">45</t>
+    <t xml:space="preserve">47</t>
   </si>
 </sst>
 </file>
@@ -571,442 +553,322 @@
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>82</v>
+        <v>71</v>
       </c>
       <c r="B12" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>83</v>
+        <v>72</v>
       </c>
       <c r="B13" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>84</v>
+        <v>74</v>
       </c>
       <c r="B14" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="B15" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="B16" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="B17" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="B18" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="B19" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="n">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="B20" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="n">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="B21" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="n">
-        <v>79</v>
+        <v>71</v>
       </c>
       <c r="B22" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="n">
-        <v>80</v>
+        <v>72</v>
       </c>
       <c r="B23" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="n">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="B24" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="n">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="B25" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="n">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="B26" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="n">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="B27" t="s">
-        <v>9</v>
+        <v>25</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="n">
-        <v>71</v>
+        <v>78</v>
       </c>
       <c r="B28" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="n">
-        <v>72</v>
+        <v>79</v>
       </c>
       <c r="B29" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="n">
-        <v>74</v>
+        <v>80</v>
       </c>
       <c r="B30" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="n">
-        <v>75</v>
+        <v>81</v>
       </c>
       <c r="B31" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="n">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="B32" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="n">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="B33" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="n">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="B34" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="n">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="B35" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="n">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="B36" t="s">
-        <v>19</v>
+        <v>9</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="n">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="B37" t="s">
-        <v>16</v>
+        <v>32</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="n">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="B38" t="s">
-        <v>5</v>
+        <v>33</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="n">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="B39" t="s">
-        <v>22</v>
+        <v>31</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="n">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="B40" t="s">
-        <v>26</v>
+        <v>34</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="n">
-        <v>71</v>
+        <v>81</v>
       </c>
       <c r="B41" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="n">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B42" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="n">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B43" t="s">
-        <v>32</v>
+        <v>20</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="n">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B44" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="n">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B45" t="s">
-        <v>9</v>
+        <v>24</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="n">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B46" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="n">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B47" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="n">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B48" t="s">
-        <v>36</v>
+        <v>6</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="n">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B49" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="n">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B50" t="s">
-        <v>38</v>
+        <v>28</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="n">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B51" t="s">
         <v>39</v>
-      </c>
-    </row>
-    <row r="52">
-      <c r="A52" t="n">
-        <v>83</v>
-      </c>
-      <c r="B52" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="53">
-      <c r="A53" t="n">
-        <v>84</v>
-      </c>
-      <c r="B53" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="54">
-      <c r="A54" t="n">
-        <v>71</v>
-      </c>
-      <c r="B54" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="55">
-      <c r="A55" t="n">
-        <v>72</v>
-      </c>
-      <c r="B55" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="56">
-      <c r="A56" t="n">
-        <v>74</v>
-      </c>
-      <c r="B56" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="57">
-      <c r="A57" t="n">
-        <v>75</v>
-      </c>
-      <c r="B57" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="58">
-      <c r="A58" t="n">
-        <v>76</v>
-      </c>
-      <c r="B58" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="59">
-      <c r="A59" t="n">
-        <v>77</v>
-      </c>
-      <c r="B59" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="60">
-      <c r="A60" t="n">
-        <v>78</v>
-      </c>
-      <c r="B60" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="61">
-      <c r="A61" t="n">
-        <v>79</v>
-      </c>
-      <c r="B61" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="62">
-      <c r="A62" t="n">
-        <v>80</v>
-      </c>
-      <c r="B62" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="63">
-      <c r="A63" t="n">
-        <v>81</v>
-      </c>
-      <c r="B63" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="64">
-      <c r="A64" t="n">
-        <v>82</v>
-      </c>
-      <c r="B64" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="65">
-      <c r="A65" t="n">
-        <v>83</v>
-      </c>
-      <c r="B65" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="66">
-      <c r="A66" t="n">
-        <v>84</v>
-      </c>
-      <c r="B66" t="s">
-        <v>45</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Proyecto desplegado en AWS Gratis
</commit_message>
<xml_diff>
--- a/Proyecto/motorR/4098796/vecinos_ofertas_sin_asignar.xlsx
+++ b/Proyecto/motorR/4098796/vecinos_ofertas_sin_asignar.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="41">
   <si>
     <t xml:space="preserve">job_id</t>
   </si>
@@ -50,6 +50,9 @@
     <t xml:space="preserve">71</t>
   </si>
   <si>
+    <t xml:space="preserve">63</t>
+  </si>
+  <si>
     <t xml:space="preserve">56</t>
   </si>
   <si>
@@ -98,7 +101,7 @@
     <t xml:space="preserve">27</t>
   </si>
   <si>
-    <t xml:space="preserve">63</t>
+    <t xml:space="preserve">61</t>
   </si>
   <si>
     <t xml:space="preserve">60</t>
@@ -553,7 +556,7 @@
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>71</v>
+        <v>82</v>
       </c>
       <c r="B12" t="s">
         <v>12</v>
@@ -561,7 +564,7 @@
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B13" t="s">
         <v>13</v>
@@ -569,7 +572,7 @@
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B14" t="s">
         <v>14</v>
@@ -577,7 +580,7 @@
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B15" t="s">
         <v>15</v>
@@ -585,7 +588,7 @@
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B16" t="s">
         <v>16</v>
@@ -593,7 +596,7 @@
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B17" t="s">
         <v>17</v>
@@ -601,7 +604,7 @@
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B18" t="s">
         <v>18</v>
@@ -609,7 +612,7 @@
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B19" t="s">
         <v>19</v>
@@ -617,7 +620,7 @@
     </row>
     <row r="20">
       <c r="A20" t="n">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B20" t="s">
         <v>20</v>
@@ -625,7 +628,7 @@
     </row>
     <row r="21">
       <c r="A21" t="n">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B21" t="s">
         <v>21</v>
@@ -633,31 +636,31 @@
     </row>
     <row r="22">
       <c r="A22" t="n">
-        <v>71</v>
+        <v>81</v>
       </c>
       <c r="B22" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="n">
-        <v>72</v>
+        <v>82</v>
       </c>
       <c r="B23" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="n">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B24" t="s">
-        <v>13</v>
+        <v>22</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="n">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="B25" t="s">
         <v>23</v>
@@ -665,167 +668,167 @@
     </row>
     <row r="26">
       <c r="A26" t="n">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B26" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="n">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B27" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="n">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B28" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="n">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B29" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="n">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B30" t="s">
-        <v>18</v>
+        <v>27</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="n">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B31" t="s">
-        <v>12</v>
+        <v>28</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="n">
-        <v>71</v>
+        <v>80</v>
       </c>
       <c r="B32" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="n">
-        <v>72</v>
+        <v>81</v>
       </c>
       <c r="B33" t="s">
-        <v>29</v>
+        <v>13</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="n">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="B34" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="n">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="B35" t="s">
-        <v>31</v>
+        <v>12</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="n">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="B36" t="s">
-        <v>9</v>
+        <v>30</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="n">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="B37" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="n">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B38" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="n">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="B39" t="s">
-        <v>31</v>
+        <v>9</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="n">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="B40" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="n">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="B41" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="n">
-        <v>71</v>
+        <v>79</v>
       </c>
       <c r="B42" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="n">
-        <v>72</v>
+        <v>80</v>
       </c>
       <c r="B43" t="s">
-        <v>20</v>
+        <v>35</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="n">
-        <v>74</v>
+        <v>81</v>
       </c>
       <c r="B44" t="s">
-        <v>29</v>
+        <v>12</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="n">
-        <v>75</v>
+        <v>82</v>
       </c>
       <c r="B45" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="n">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="B46" t="s">
         <v>36</v>
@@ -833,42 +836,82 @@
     </row>
     <row r="47">
       <c r="A47" t="n">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="B47" t="s">
-        <v>37</v>
+        <v>21</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="n">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="B48" t="s">
-        <v>6</v>
+        <v>30</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="n">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="B49" t="s">
-        <v>38</v>
+        <v>25</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="n">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="B50" t="s">
-        <v>28</v>
+        <v>37</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="n">
+        <v>77</v>
+      </c>
+      <c r="B51" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="n">
+        <v>78</v>
+      </c>
+      <c r="B52" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="n">
+        <v>79</v>
+      </c>
+      <c r="B53" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="n">
+        <v>80</v>
+      </c>
+      <c r="B54" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="n">
         <v>81</v>
       </c>
-      <c r="B51" t="s">
-        <v>39</v>
+      <c r="B55" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="n">
+        <v>82</v>
+      </c>
+      <c r="B56" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
añadida base de datos
</commit_message>
<xml_diff>
--- a/Proyecto/motorR/4098796/vecinos_ofertas_sin_asignar.xlsx
+++ b/Proyecto/motorR/4098796/vecinos_ofertas_sin_asignar.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="47">
   <si>
     <t xml:space="preserve">job_id</t>
   </si>
@@ -50,6 +50,12 @@
     <t xml:space="preserve">71</t>
   </si>
   <si>
+    <t xml:space="preserve">84</t>
+  </si>
+  <si>
+    <t xml:space="preserve">83</t>
+  </si>
+  <si>
     <t xml:space="preserve">56</t>
   </si>
   <si>
@@ -80,6 +86,9 @@
     <t xml:space="preserve">55</t>
   </si>
   <si>
+    <t xml:space="preserve">6</t>
+  </si>
+  <si>
     <t xml:space="preserve">74</t>
   </si>
   <si>
@@ -98,6 +107,12 @@
     <t xml:space="preserve">27</t>
   </si>
   <si>
+    <t xml:space="preserve">8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3</t>
+  </si>
+  <si>
     <t xml:space="preserve">63</t>
   </si>
   <si>
@@ -107,18 +122,21 @@
     <t xml:space="preserve">72</t>
   </si>
   <si>
+    <t xml:space="preserve">13</t>
+  </si>
+  <si>
+    <t xml:space="preserve">44</t>
+  </si>
+  <si>
     <t xml:space="preserve">30</t>
   </si>
   <si>
-    <t xml:space="preserve">13</t>
-  </si>
-  <si>
-    <t xml:space="preserve">44</t>
-  </si>
-  <si>
     <t xml:space="preserve">51</t>
   </si>
   <si>
+    <t xml:space="preserve">12</t>
+  </si>
+  <si>
     <t xml:space="preserve">41</t>
   </si>
   <si>
@@ -132,6 +150,9 @@
   </si>
   <si>
     <t xml:space="preserve">47</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2</t>
   </si>
 </sst>
 </file>
@@ -553,7 +574,7 @@
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>71</v>
+        <v>83</v>
       </c>
       <c r="B12" t="s">
         <v>12</v>
@@ -561,7 +582,7 @@
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>72</v>
+        <v>84</v>
       </c>
       <c r="B13" t="s">
         <v>13</v>
@@ -569,7 +590,7 @@
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B14" t="s">
         <v>14</v>
@@ -577,7 +598,7 @@
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="B15" t="s">
         <v>15</v>
@@ -585,7 +606,7 @@
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B16" t="s">
         <v>16</v>
@@ -593,7 +614,7 @@
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B17" t="s">
         <v>17</v>
@@ -601,7 +622,7 @@
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B18" t="s">
         <v>18</v>
@@ -609,7 +630,7 @@
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B19" t="s">
         <v>19</v>
@@ -617,7 +638,7 @@
     </row>
     <row r="20">
       <c r="A20" t="n">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B20" t="s">
         <v>20</v>
@@ -625,7 +646,7 @@
     </row>
     <row r="21">
       <c r="A21" t="n">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B21" t="s">
         <v>21</v>
@@ -633,47 +654,47 @@
     </row>
     <row r="22">
       <c r="A22" t="n">
-        <v>71</v>
+        <v>80</v>
       </c>
       <c r="B22" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="n">
-        <v>72</v>
+        <v>81</v>
       </c>
       <c r="B23" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="n">
-        <v>74</v>
+        <v>83</v>
       </c>
       <c r="B24" t="s">
-        <v>13</v>
+        <v>24</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="n">
-        <v>75</v>
+        <v>84</v>
       </c>
       <c r="B25" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="n">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="B26" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="n">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="B27" t="s">
         <v>25</v>
@@ -681,79 +702,79 @@
     </row>
     <row r="28">
       <c r="A28" t="n">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="B28" t="s">
-        <v>26</v>
+        <v>15</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="n">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="B29" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="n">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="B30" t="s">
-        <v>18</v>
+        <v>27</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="n">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="B31" t="s">
-        <v>12</v>
+        <v>28</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="n">
-        <v>71</v>
+        <v>78</v>
       </c>
       <c r="B32" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="n">
-        <v>72</v>
+        <v>79</v>
       </c>
       <c r="B33" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="n">
-        <v>74</v>
+        <v>80</v>
       </c>
       <c r="B34" t="s">
-        <v>30</v>
+        <v>20</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="n">
-        <v>75</v>
+        <v>81</v>
       </c>
       <c r="B35" t="s">
-        <v>31</v>
+        <v>14</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="n">
-        <v>76</v>
+        <v>83</v>
       </c>
       <c r="B36" t="s">
-        <v>9</v>
+        <v>31</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="n">
-        <v>77</v>
+        <v>84</v>
       </c>
       <c r="B37" t="s">
         <v>32</v>
@@ -761,7 +782,7 @@
     </row>
     <row r="38">
       <c r="A38" t="n">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="B38" t="s">
         <v>33</v>
@@ -769,106 +790,186 @@
     </row>
     <row r="39">
       <c r="A39" t="n">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="B39" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="n">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="B40" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="n">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="B41" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="n">
-        <v>71</v>
+        <v>76</v>
       </c>
       <c r="B42" t="s">
-        <v>35</v>
+        <v>9</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="n">
-        <v>72</v>
+        <v>77</v>
       </c>
       <c r="B43" t="s">
-        <v>20</v>
+        <v>36</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="n">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="B44" t="s">
-        <v>29</v>
+        <v>37</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="n">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="B45" t="s">
-        <v>24</v>
+        <v>38</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="n">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="B46" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="n">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="B47" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="n">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="B48" t="s">
-        <v>6</v>
+        <v>32</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="n">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="B49" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="n">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="B50" t="s">
-        <v>28</v>
+        <v>41</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="n">
+        <v>72</v>
+      </c>
+      <c r="B51" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="n">
+        <v>74</v>
+      </c>
+      <c r="B52" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="n">
+        <v>75</v>
+      </c>
+      <c r="B53" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="n">
+        <v>76</v>
+      </c>
+      <c r="B54" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="n">
+        <v>77</v>
+      </c>
+      <c r="B55" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="n">
+        <v>78</v>
+      </c>
+      <c r="B56" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="n">
+        <v>79</v>
+      </c>
+      <c r="B57" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="n">
+        <v>80</v>
+      </c>
+      <c r="B58" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="n">
         <v>81</v>
       </c>
-      <c r="B51" t="s">
-        <v>39</v>
+      <c r="B59" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="n">
+        <v>83</v>
+      </c>
+      <c r="B60" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="n">
+        <v>84</v>
+      </c>
+      <c r="B61" t="s">
+        <v>46</v>
       </c>
     </row>
   </sheetData>

</xml_diff>